<commit_message>
added SEs to 'cookstoves'
</commit_message>
<xml_diff>
--- a/data/2a_causal_estimates_papers/uncorrected_vJK/cookstoves.xlsx
+++ b/data/2a_causal_estimates_papers/uncorrected_vJK/cookstoves.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackkelly/Opportunity Insights Dropbox/Jack Kelly/Regulation/code_files/2a_causal_estimates_papers/uncorrected_vJK/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcchen\Documents\GitHub\mvpf-climate\data\2a_causal_estimates_papers\uncorrected_vJK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F73A99-4A35-CD45-876B-7ABE629862C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0157713F-B0FB-41FD-B6A7-17CA4F9E077C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11000" yWindow="2000" windowWidth="28800" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wrapper_ready" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -168,7 +166,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1065,12 +1063,15 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="19.296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1116,6 +1117,9 @@
         <f>raw_data!B2</f>
         <v>6.0000000000000001E-3</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
       <c r="H2">
         <v>1</v>
       </c>
@@ -1123,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1131,8 +1135,11 @@
         <f>raw_data!B3</f>
         <v>0.54500000000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1140,8 +1147,11 @@
         <f>calculations!C2</f>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1164,21 +1174,21 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="8.6640625" style="2"/>
+    <col min="1" max="1" width="27.69921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="8.69921875" style="2"/>
     <col min="8" max="8" width="12" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" customWidth="1"/>
-    <col min="11" max="16384" width="8.6640625" style="2"/>
+    <col min="10" max="10" width="27.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.69921875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="27.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1214,7 +1224,7 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="42">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1231,7 +1241,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1243,7 +1253,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="27.6">
       <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
@@ -1254,7 +1264,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="27.6">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -1278,17 +1288,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="14.4">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="83.4">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1296,23 +1306,23 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="14.4">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="14.4">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="14.4">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="14.4">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
     </row>
@@ -1329,12 +1339,12 @@
   <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="28.8">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -1351,7 +1361,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="14.4">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1365,7 +1375,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="2"/>
     </row>
   </sheetData>
@@ -1384,15 +1394,15 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="24.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="2"/>
+    <col min="2" max="2" width="45.69921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.69921875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1403,7 +1413,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="27.6">
       <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
@@ -1413,17 +1423,17 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>

</xml_diff>